<commit_message>
forgot to add BOM
</commit_message>
<xml_diff>
--- a/microstim/microstim_BOM.xlsx
+++ b/microstim/microstim_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -286,12 +286,6 @@
     <t xml:space="preserve">U14,U15</t>
   </si>
   <si>
-    <t xml:space="preserve">LT1167</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT1167CS8#PBF-ND </t>
-  </si>
-  <si>
     <t xml:space="preserve">INA826</t>
   </si>
   <si>
@@ -308,9 +302,6 @@
   </si>
   <si>
     <t xml:space="preserve">DG509BEY-T1-E3CT-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(NOT PIN COMPATIBLE)</t>
   </si>
   <si>
     <t xml:space="preserve">U6</t>
@@ -337,6 +328,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -358,6 +350,7 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -428,17 +421,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
@@ -1108,20 +1101,11 @@
         <v>89</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>6.54</v>
+        <v>2.81</v>
       </c>
       <c r="H25" s="0" t="n">
         <f aca="false">G25*D25</f>
-        <v>13.08</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L25" s="0" t="n">
-        <v>2.81</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,19 +1113,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>2.43</v>
@@ -1150,28 +1134,25 @@
         <f aca="false">G26*D26</f>
         <v>4.86</v>
       </c>
-      <c r="J26" s="0" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>1.76</v>
@@ -1184,7 +1165,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H29" s="0" t="n">
         <f aca="false">SUM(H2:H27)</f>
-        <v>115.25</v>
+        <v>107.79</v>
       </c>
     </row>
   </sheetData>
@@ -1211,10 +1192,9 @@
     <hyperlink ref="F22" r:id="rId20" display="P20292CT-ND "/>
     <hyperlink ref="F23" r:id="rId21" display="MCT0603-1.00K-CFCT-ND "/>
     <hyperlink ref="F24" r:id="rId22" display="AD8276ARZ-ND "/>
-    <hyperlink ref="F25" r:id="rId23" display="LT1167CS8#PBF-ND "/>
-    <hyperlink ref="K25" r:id="rId24" display="296-30238-1-ND "/>
-    <hyperlink ref="F26" r:id="rId25" display="DG509BEY-T1-E3CT-ND "/>
-    <hyperlink ref="F27" r:id="rId26" display="AD1582ARTZREEL7CT-ND "/>
+    <hyperlink ref="F25" r:id="rId23" display="296-30238-1-ND "/>
+    <hyperlink ref="F26" r:id="rId24" display="DG509BEY-T1-E3CT-ND "/>
+    <hyperlink ref="F27" r:id="rId25" display="AD1582ARTZREEL7CT-ND "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
bunch of small fixes to board. havent yet regenerated gerbers. also added beginnings of teensy controller code.
</commit_message>
<xml_diff>
--- a/microstim/microstim_BOM.xlsx
+++ b/microstim/microstim_BOM.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="microstim" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="microstim_BOM_new" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="95">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -40,16 +40,67 @@
     <t xml:space="preserve">Supplier and ref</t>
   </si>
   <si>
-    <t xml:space="preserve">Cost per unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplier+ref</t>
+    <t xml:space="preserve">Alternative part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1,SW2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_SPST_PTS645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_Push</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CKN9112CT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_1206_3216Metric_Pad1.42x1.75mm_HandSolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1376-1-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOIC-16W_7.5x10.3mm_P1.27mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO7341C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-47779-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6,C2,C7,C8,C12,C14,C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-1019-1-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8,R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P20292CT-ND </t>
   </si>
   <si>
     <t xml:space="preserve">U10</t>
@@ -64,27 +115,6 @@
     <t xml:space="preserve">AD7321BRUZ-REEL7CT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C_0603_1608Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-1376-1-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2,C6,C7,C8,C12,C14,C4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-1019-1-ND </t>
-  </si>
-  <si>
     <t xml:space="preserve">C3,C5,C9,C11,C13,C15,C16,C17,C18,C19,C20,C21,C22,C23,C24,C25,C31,C33,C36,C40</t>
   </si>
   <si>
@@ -139,18 +169,6 @@
     <t xml:space="preserve">3296Y-102LF-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">SW1,SW2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW_PUSH_6mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW_Push</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKN9112CT-ND </t>
-  </si>
-  <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
@@ -196,24 +214,12 @@
     <t xml:space="preserve">U5</t>
   </si>
   <si>
-    <t xml:space="preserve">SOIC-16W_7.5x10.3mm_P1.27mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">ISO7760</t>
   </si>
   <si>
     <t xml:space="preserve">296-48142-1-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISO7341C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-47779-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">U8</t>
   </si>
   <si>
@@ -235,18 +241,9 @@
     <t xml:space="preserve">MCP4922-E/SL-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">REF**,REF**,REF**,REF**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MountingHole_3.5mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">R1,R2,R4,R5</t>
   </si>
   <si>
-    <t xml:space="preserve">R_0603_1608Metric</t>
-  </si>
-  <si>
     <t xml:space="preserve">3k</t>
   </si>
   <si>
@@ -259,15 +256,6 @@
     <t xml:space="preserve">P249BLCT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">R7,R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P20292CT-ND </t>
-  </si>
-  <si>
     <t xml:space="preserve">R9,R13</t>
   </si>
   <si>
@@ -283,7 +271,7 @@
     <t xml:space="preserve">AD8276ARZ-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">U14,U15</t>
+    <t xml:space="preserve">U14,U11</t>
   </si>
   <si>
     <t xml:space="preserve">INA826</t>
@@ -304,6 +292,9 @@
     <t xml:space="preserve">DG509BEY-T1-E3CT-ND </t>
   </si>
   <si>
+    <t xml:space="preserve">DG409DY-T1-E3CT-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">U6</t>
   </si>
   <si>
@@ -314,15 +305,6 @@
   </si>
   <si>
     <t xml:space="preserve">AD1582ARTZREEL7CT-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN HEADER FEMALE 24POS.1" TIN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female headers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S7022-ND </t>
   </si>
 </sst>
 </file>
@@ -337,7 +319,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -411,16 +392,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -445,17 +422,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
@@ -481,17 +458,8 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,26 +467,26 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="G2" s="0" t="n">
-        <v>7.84</v>
+        <v>0.16</v>
       </c>
       <c r="H2" s="0" t="n">
         <f aca="false">G2*D2</f>
-        <v>7.84</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,19 +494,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>0.4</v>
@@ -553,26 +521,26 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G4" s="0" t="n">
-        <v>0.1</v>
+        <v>4.32</v>
       </c>
       <c r="H4" s="0" t="n">
         <f aca="false">G4*D4</f>
-        <v>0.7</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,26 +548,26 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G5" s="0" t="n">
-        <v>0.038</v>
+        <v>0.1</v>
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">G5*D5</f>
-        <v>0.76</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,13 +575,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>25</v>
@@ -622,11 +590,11 @@
         <v>26</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">G6*D6</f>
-        <v>0.1</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,7 +608,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>29</v>
@@ -649,11 +617,11 @@
         <v>30</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>2.16</v>
+        <v>7.84</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">G7*D7</f>
-        <v>12.96</v>
+        <v>7.84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,23 +632,23 @@
         <v>31</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="0" t="n">
-        <v>0.46</v>
+        <v>0.038</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">G8*D8</f>
-        <v>2.76</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,26 +656,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="G9" s="0" t="n">
-        <v>2.41</v>
+        <v>0.1</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">G9*D9</f>
-        <v>4.82</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,26 +683,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="G10" s="0" t="n">
-        <v>0.16</v>
+        <v>2.16</v>
       </c>
       <c r="H10" s="0" t="n">
         <f aca="false">G10*D10</f>
-        <v>0.32</v>
+        <v>12.96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -742,26 +710,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G11" s="0" t="n">
-        <v>31.25</v>
+        <v>0.46</v>
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">G11*D11</f>
-        <v>31.25</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,26 +737,26 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="G12" s="0" t="n">
-        <v>11.21</v>
+        <v>2.41</v>
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">G12*D12</f>
-        <v>11.21</v>
+        <v>4.82</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,26 +764,26 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="G13" s="0" t="n">
-        <v>0.48</v>
+        <v>31.25</v>
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">G13*D13</f>
-        <v>0.48</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,26 +791,26 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="G14" s="0" t="n">
-        <v>0.44</v>
+        <v>11.21</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">G14*D14</f>
-        <v>0.44</v>
+        <v>11.21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,26 +818,26 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="G15" s="0" t="n">
-        <v>4.44</v>
+        <v>0.48</v>
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">G15*D15</f>
-        <v>4.44</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,26 +845,26 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G16" s="0" t="n">
-        <v>4.32</v>
+        <v>0.44</v>
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">G16*D16</f>
-        <v>4.32</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,26 +872,26 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G17" s="0" t="n">
-        <v>0.41</v>
+        <v>4.44</v>
       </c>
       <c r="H17" s="0" t="n">
         <f aca="false">G17*D17</f>
-        <v>0.41</v>
+        <v>4.44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,26 +899,26 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="G18" s="0" t="n">
-        <v>2.7</v>
+        <v>0.41</v>
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">G18*D18</f>
-        <v>2.7</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,16 +926,26 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>72</v>
+      <c r="G19" s="0" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">G19*D19</f>
+        <v>2.7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,16 +956,16 @@
         <v>73</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E20" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>0.8</v>
@@ -1002,10 +980,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>2</v>
@@ -1014,7 +992,7 @@
         <v>250</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>0.13</v>
@@ -1029,19 +1007,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0.18</v>
@@ -1056,26 +1034,26 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0.18</v>
+        <v>2.73</v>
       </c>
       <c r="H23" s="0" t="n">
         <f aca="false">G23*D23</f>
-        <v>0.36</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,26 +1061,26 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="G24" s="0" t="n">
-        <v>2.73</v>
+        <v>2.81</v>
       </c>
       <c r="H24" s="0" t="n">
         <f aca="false">G24*D24</f>
-        <v>5.46</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,10 +1088,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>2</v>
@@ -1125,11 +1103,14 @@
         <v>89</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>2.81</v>
+        <v>2.43</v>
       </c>
       <c r="H25" s="0" t="n">
         <f aca="false">G25*D25</f>
-        <v>5.62</v>
+        <v>4.86</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,110 +1118,56 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>2.43</v>
+        <v>1.76</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">G26*D26</f>
-        <v>4.86</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="0" t="n">
         <v>1.76</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <f aca="false">G27*D27</f>
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <v>1.37</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <f aca="false">G28*D28</f>
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="0" t="n">
-        <f aca="false">SUM(H2:H28)</f>
-        <v>110.53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="AD7321BRUZ-REEL7CT-ND "/>
+    <hyperlink ref="F2" r:id="rId1" display="CKN9112CT-ND "/>
     <hyperlink ref="F3" r:id="rId2" display="311-1376-1-ND "/>
-    <hyperlink ref="F4" r:id="rId3" display="1276-1019-1-ND "/>
-    <hyperlink ref="F5" r:id="rId4" display="CL10F104ZO8NNNC"/>
-    <hyperlink ref="F6" r:id="rId5" display="732-7988-1-ND "/>
-    <hyperlink ref="F7" r:id="rId6" display="A97594-ND "/>
-    <hyperlink ref="F8" r:id="rId7" display="277-1721-ND "/>
-    <hyperlink ref="F9" r:id="rId8" display="3296Y-102LF-ND "/>
-    <hyperlink ref="F10" r:id="rId9" display="CKN9112CT-ND "/>
-    <hyperlink ref="F11" r:id="rId10" display="1568-1464-ND "/>
-    <hyperlink ref="F12" r:id="rId11" display="445-2465-ND "/>
-    <hyperlink ref="F13" r:id="rId12" display="MC78L05ACDXCT-ND "/>
-    <hyperlink ref="F14" r:id="rId13" display="MC78L12ABDGOS-ND "/>
-    <hyperlink ref="F15" r:id="rId14" display="296-48142-1-ND "/>
-    <hyperlink ref="F16" r:id="rId15" display="296-47779-1-ND"/>
-    <hyperlink ref="F17" r:id="rId16" display="MC79L12ACDR2GOSCT-ND "/>
-    <hyperlink ref="F18" r:id="rId17" display="MCP4922-E/SL-ND "/>
-    <hyperlink ref="F20" r:id="rId18" display="P3.0KBECT-ND "/>
-    <hyperlink ref="F21" r:id="rId19" display="P249BLCT-ND "/>
-    <hyperlink ref="F22" r:id="rId20" display="P20292CT-ND "/>
-    <hyperlink ref="F23" r:id="rId21" display="MCT0603-1.00K-CFCT-ND "/>
-    <hyperlink ref="F24" r:id="rId22" display="AD8276ARZ-ND "/>
-    <hyperlink ref="F25" r:id="rId23" display="296-30238-1-ND "/>
-    <hyperlink ref="F26" r:id="rId24" display="DG509BEY-T1-E3CT-ND "/>
-    <hyperlink ref="F27" r:id="rId25" display="AD1582ARTZREEL7CT-ND "/>
-    <hyperlink ref="F28" r:id="rId26" display="S7022-ND "/>
+    <hyperlink ref="F4" r:id="rId3" display="296-47779-1-ND"/>
+    <hyperlink ref="F5" r:id="rId4" display="1276-1019-1-ND "/>
+    <hyperlink ref="F6" r:id="rId5" display="P20292CT-ND "/>
+    <hyperlink ref="F7" r:id="rId6" display="AD7321BRUZ-REEL7CT-ND "/>
+    <hyperlink ref="F8" r:id="rId7" display="CL10F104ZO8NNNC"/>
+    <hyperlink ref="F9" r:id="rId8" display="732-7988-1-ND "/>
+    <hyperlink ref="F10" r:id="rId9" display="A97594-ND "/>
+    <hyperlink ref="F11" r:id="rId10" display="277-1721-ND "/>
+    <hyperlink ref="F12" r:id="rId11" display="3296Y-102LF-ND "/>
+    <hyperlink ref="F13" r:id="rId12" display="1568-1464-ND "/>
+    <hyperlink ref="F14" r:id="rId13" display="445-2465-ND "/>
+    <hyperlink ref="F15" r:id="rId14" display="MC78L05ACDXCT-ND "/>
+    <hyperlink ref="F16" r:id="rId15" display="MC78L12ABDGOS-ND "/>
+    <hyperlink ref="F17" r:id="rId16" display="296-48142-1-ND "/>
+    <hyperlink ref="F18" r:id="rId17" display="MC79L12ACDR2GOSCT-ND "/>
+    <hyperlink ref="F19" r:id="rId18" display="MCP4922-E/SL-ND "/>
+    <hyperlink ref="F20" r:id="rId19" display="P3.0KBECT-ND "/>
+    <hyperlink ref="F21" r:id="rId20" display="P249BLCT-ND "/>
+    <hyperlink ref="F22" r:id="rId21" display="MCT0603-1.00K-CFCT-ND "/>
+    <hyperlink ref="F23" r:id="rId22" display="AD8276ARZ-ND "/>
+    <hyperlink ref="F24" r:id="rId23" display="296-30238-1-ND "/>
+    <hyperlink ref="F25" r:id="rId24" display="DG509BEY-T1-E3CT-ND "/>
+    <hyperlink ref="I25" r:id="rId25" display="DG409DY-T1-E3CT-ND "/>
+    <hyperlink ref="F26" r:id="rId26" display="AD1582ARTZREEL7CT-ND "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>